<commit_message>
Clean up, add repo name
</commit_message>
<xml_diff>
--- a/ESP32 Plotter Controller JLCPCB-LCSC BOM.xlsx
+++ b/ESP32 Plotter Controller JLCPCB-LCSC BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/635c63a8a9b49b7f/Code/ESP32_Plotter_Controller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="462" documentId="8_{D55F54B1-64B4-46E1-9F7C-A5FE78793489}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1887C89F-6804-488A-9404-C36BEA60EDCA}"/>
+  <xr:revisionPtr revIDLastSave="521" documentId="8_{D55F54B1-64B4-46E1-9F7C-A5FE78793489}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A5CE3CC6-27FB-43B9-AF21-B649572EF67A}"/>
   <bookViews>
     <workbookView xWindow="-37580" yWindow="-12810" windowWidth="37690" windowHeight="21820" xr2:uid="{9EA36A07-8613-46A5-ADBE-75DCC70AAE57}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="159">
   <si>
     <t>ESP32 Plotter Controller parts cross check</t>
   </si>
@@ -417,9 +417,6 @@
     <t>C280412</t>
   </si>
   <si>
-    <t>Order BOM</t>
-  </si>
-  <si>
     <t>LCSC Part No:</t>
   </si>
   <si>
@@ -484,13 +481,43 @@
   </si>
   <si>
     <t>47uF 25v SMT Elec</t>
+  </si>
+  <si>
+    <t>CP_ELEC_6.3x5.7</t>
+  </si>
+  <si>
+    <t>C176688</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>47uF</t>
+  </si>
+  <si>
+    <t>Y Stepper resivoir</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>X Stepper resivoir</t>
+  </si>
+  <si>
+    <t>Line Cost</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Component Order BOM (lcsc.com)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -504,25 +531,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -534,17 +549,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -857,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC7673F-706C-49DA-BE28-CCAA818D7664}">
-  <dimension ref="B2:M77"/>
+  <dimension ref="B2:M83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74:G74"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -869,7 +881,7 @@
     <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1453,7 +1465,7 @@
         <v>60</v>
       </c>
       <c r="K23">
-        <v>6.2199999999999998E-2</v>
+        <v>0.1119</v>
       </c>
       <c r="M23">
         <v>1</v>
@@ -1752,7 +1764,7 @@
         <v>5.2600000000000001E-2</v>
       </c>
       <c r="J35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K35">
         <v>1.6299999999999999E-2</v>
@@ -1851,94 +1863,85 @@
         <v>1</v>
       </c>
     </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" t="s">
+        <v>152</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E39" t="s">
+        <v>153</v>
+      </c>
+      <c r="F39" t="s">
+        <v>61</v>
+      </c>
+      <c r="J39" t="s">
+        <v>150</v>
+      </c>
+      <c r="K39">
+        <v>0.1016</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+    </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>100</v>
+        <v>154</v>
       </c>
       <c r="C40" t="s">
-        <v>103</v>
+        <v>152</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="E40" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
       <c r="F40" t="s">
         <v>61</v>
       </c>
-      <c r="G40" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40">
-        <v>1.2999999999999999E-3</v>
-      </c>
       <c r="J40" t="s">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="K40">
-        <v>1.2999999999999999E-3</v>
+        <v>0.1016</v>
       </c>
       <c r="M40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>104</v>
-      </c>
-      <c r="C41" t="s">
-        <v>103</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E41" t="s">
-        <v>105</v>
-      </c>
-      <c r="F41" t="s">
-        <v>61</v>
-      </c>
-      <c r="G41" t="s">
-        <v>11</v>
-      </c>
-      <c r="H41">
-        <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="J41" t="s">
-        <v>102</v>
-      </c>
-      <c r="K41">
-        <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="M41">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C42" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E42" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="F42" t="s">
         <v>61</v>
       </c>
       <c r="G42" t="s">
-        <v>27</v>
+        <v>11</v>
+      </c>
+      <c r="H42">
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="J42" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="K42">
-        <v>1.5E-3</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="M42">
         <v>1</v>
@@ -1946,54 +1949,89 @@
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C43" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E43" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F43" t="s">
         <v>61</v>
       </c>
       <c r="G43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="J43" t="s">
+        <v>102</v>
+      </c>
+      <c r="K43">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C44" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E44" t="s">
+        <v>109</v>
+      </c>
+      <c r="F44" t="s">
+        <v>61</v>
+      </c>
+      <c r="G44" t="s">
         <v>27</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J44" t="s">
         <v>108</v>
       </c>
-      <c r="K43">
+      <c r="K44">
         <v>1.5E-3</v>
       </c>
-      <c r="M43">
+      <c r="M44">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C45" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="E45" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="F45" t="s">
         <v>61</v>
       </c>
+      <c r="G45" t="s">
+        <v>27</v>
+      </c>
       <c r="J45" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="K45">
-        <v>0.23200000000000001</v>
+        <v>1.5E-3</v>
       </c>
       <c r="M45">
         <v>1</v>
@@ -2001,172 +2039,215 @@
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" t="s">
+        <v>113</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E47" t="s">
+        <v>86</v>
+      </c>
+      <c r="F47" t="s">
+        <v>61</v>
+      </c>
+      <c r="J47" t="s">
+        <v>115</v>
+      </c>
+      <c r="K47">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
         <v>122</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C49" t="s">
         <v>124</v>
       </c>
-      <c r="K47">
+      <c r="K49">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
         <v>123</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C50" t="s">
         <v>124</v>
       </c>
-      <c r="K48">
+      <c r="K50">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="K50">
-        <f>SUM(K5:K48)</f>
-        <v>12.593700000000002</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B53" t="s">
-        <v>127</v>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K52">
+        <f>SUM(K5:K50)</f>
+        <v>12.846600000000002</v>
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>128</v>
-      </c>
-      <c r="C55" t="s">
-        <v>131</v>
-      </c>
-      <c r="D55" t="s">
-        <v>129</v>
-      </c>
-      <c r="E55" t="s">
-        <v>3</v>
-      </c>
-      <c r="F55" t="s">
-        <v>2</v>
-      </c>
-      <c r="G55" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B56" t="s">
-        <v>39</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" t="s">
-        <v>75</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>120</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
+        <v>127</v>
+      </c>
+      <c r="C57" t="s">
+        <v>130</v>
       </c>
       <c r="D57" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="E57" t="s">
-        <v>133</v>
+        <v>3</v>
+      </c>
+      <c r="F57" t="s">
+        <v>2</v>
+      </c>
+      <c r="G57" t="s">
+        <v>129</v>
+      </c>
+      <c r="H57" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>137</v>
+        <v>8</v>
       </c>
       <c r="E58" t="s">
-        <v>66</v>
+        <v>75</v>
+      </c>
+      <c r="G58">
+        <v>0.14879999999999999</v>
+      </c>
+      <c r="H58">
+        <f>G58*C58</f>
+        <v>0.14879999999999999</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>31</v>
+        <v>120</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E59" t="s">
-        <v>68</v>
+        <v>132</v>
+      </c>
+      <c r="G59">
+        <v>0.1023</v>
+      </c>
+      <c r="H59">
+        <f t="shared" ref="H59:H80" si="0">G59*C59</f>
+        <v>0.1023</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D60" t="s">
-        <v>28</v>
+        <v>136</v>
       </c>
       <c r="E60" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+      <c r="G60">
+        <v>1.2E-2</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="0"/>
+        <v>2.4E-2</v>
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C61">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>134</v>
+        <v>19</v>
       </c>
       <c r="E61" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="G61">
+        <v>3.4200000000000001E-2</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="0"/>
+        <v>3.4200000000000001E-2</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>136</v>
+        <v>28</v>
       </c>
       <c r="E62" t="s">
-        <v>71</v>
+        <v>69</v>
+      </c>
+      <c r="G62">
+        <v>3.4200000000000001E-2</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="0"/>
+        <v>3.4200000000000001E-2</v>
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
       <c r="E63" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="G63">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="0"/>
+        <v>9.7999999999999997E-3</v>
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C64">
         <v>2</v>
@@ -2175,213 +2256,391 @@
         <v>135</v>
       </c>
       <c r="E64" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="G64">
+        <v>1.9900000000000001E-2</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="0"/>
+        <v>3.9800000000000002E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C65">
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="E65" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="G65">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="0"/>
+        <v>0.34499999999999997</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C66">
         <v>2</v>
       </c>
       <c r="D66" t="s">
-        <v>55</v>
+        <v>134</v>
       </c>
       <c r="E66" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="G66">
+        <v>1.89E-2</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="0"/>
+        <v>3.78E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="C67">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>147</v>
+        <v>34</v>
       </c>
       <c r="E67" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="G67">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="0"/>
+        <v>0.17799999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C68">
         <v>2</v>
       </c>
       <c r="D68" t="s">
+        <v>55</v>
+      </c>
+      <c r="E68" t="s">
+        <v>76</v>
+      </c>
+      <c r="G68">
+        <v>0.1119</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="0"/>
+        <v>0.2238</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>60</v>
+      </c>
+      <c r="C69">
+        <v>4</v>
+      </c>
+      <c r="D69" t="s">
         <v>146</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E69" t="s">
+        <v>77</v>
+      </c>
+      <c r="G69">
+        <v>0.1119</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="0"/>
+        <v>0.4476</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>62</v>
+      </c>
+      <c r="C70">
+        <v>2</v>
+      </c>
+      <c r="D70" t="s">
+        <v>145</v>
+      </c>
+      <c r="E70" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B69" t="s">
+      <c r="G70">
+        <v>7.2300000000000003E-2</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="0"/>
+        <v>0.14460000000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>119</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71" t="s">
+        <v>116</v>
+      </c>
+      <c r="E71" t="s">
+        <v>118</v>
+      </c>
+      <c r="F71" t="s">
+        <v>117</v>
+      </c>
+      <c r="G71">
+        <v>0.2268</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="0"/>
+        <v>0.2268</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
         <v>81</v>
       </c>
-      <c r="C69">
+      <c r="C72">
         <v>2</v>
       </c>
-      <c r="D69" t="s">
-        <v>132</v>
-      </c>
-      <c r="E69" t="s">
+      <c r="D72" t="s">
+        <v>131</v>
+      </c>
+      <c r="E72" t="s">
         <v>82</v>
       </c>
-      <c r="F69" t="s">
+      <c r="F72" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B70" t="s">
+      <c r="G72">
+        <v>4.0399999999999998E-2</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="0"/>
+        <v>8.0799999999999997E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
         <v>126</v>
       </c>
-      <c r="C70">
-        <v>1</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73" t="s">
         <v>85</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E73" t="s">
         <v>87</v>
       </c>
-      <c r="F70" t="s">
+      <c r="F73" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B71" t="s">
-        <v>145</v>
-      </c>
-      <c r="C71">
-        <v>1</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="G73">
+        <v>0.1255</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="0"/>
+        <v>0.1255</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>144</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74" t="s">
         <v>88</v>
       </c>
-      <c r="E71">
-        <v>805</v>
-      </c>
-      <c r="F71" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B72" t="s">
+      <c r="E74" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F74" t="s">
+        <v>137</v>
+      </c>
+      <c r="G74">
+        <v>1.6299999999999999E-2</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="0"/>
+        <v>1.6299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
         <v>94</v>
       </c>
-      <c r="C72">
-        <v>1</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75" t="s">
         <v>91</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E75" t="s">
         <v>92</v>
       </c>
-      <c r="F72" t="s">
+      <c r="F75" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B73" t="s">
+      <c r="G75">
+        <v>0.30330000000000001</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="0"/>
+        <v>0.30330000000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
         <v>98</v>
-      </c>
-      <c r="C73">
-        <v>2</v>
-      </c>
-      <c r="D73" t="s">
-        <v>139</v>
-      </c>
-      <c r="E73">
-        <v>603</v>
-      </c>
-      <c r="F73" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B74" s="2"/>
-      <c r="C74" s="2">
-        <v>2</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="G74" s="2"/>
-    </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B75" t="s">
-        <v>102</v>
-      </c>
-      <c r="C75">
-        <v>2</v>
-      </c>
-      <c r="D75" t="s">
-        <v>141</v>
-      </c>
-      <c r="E75">
-        <v>603</v>
-      </c>
-      <c r="F75" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B76" t="s">
-        <v>108</v>
       </c>
       <c r="C76">
         <v>2</v>
       </c>
       <c r="D76" t="s">
+        <v>138</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F76" t="s">
+        <v>139</v>
+      </c>
+      <c r="G76">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="0"/>
+        <v>6.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>150</v>
+      </c>
+      <c r="C77">
+        <v>2</v>
+      </c>
+      <c r="D77" t="s">
+        <v>147</v>
+      </c>
+      <c r="E77" t="s">
+        <v>149</v>
+      </c>
+      <c r="F77" t="s">
+        <v>148</v>
+      </c>
+      <c r="G77">
+        <v>0.1016</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="0"/>
+        <v>0.20319999999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>102</v>
+      </c>
+      <c r="C78">
+        <v>2</v>
+      </c>
+      <c r="D78" t="s">
+        <v>140</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F78" t="s">
+        <v>103</v>
+      </c>
+      <c r="G78">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="0"/>
+        <v>2.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>108</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s">
+        <v>141</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F79" t="s">
         <v>142</v>
       </c>
-      <c r="E76">
-        <v>603</v>
-      </c>
-      <c r="F76" t="s">
+      <c r="G79">
+        <v>1.5E-3</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="0"/>
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>115</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>112</v>
+      </c>
+      <c r="E80" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B77" t="s">
-        <v>115</v>
-      </c>
-      <c r="C77">
-        <v>1</v>
-      </c>
-      <c r="D77" t="s">
-        <v>112</v>
-      </c>
-      <c r="E77" t="s">
-        <v>144</v>
-      </c>
-      <c r="F77" t="s">
+      <c r="F80" t="s">
         <v>113</v>
+      </c>
+      <c r="G80">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="0"/>
+        <v>0.23200000000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H82" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="83" spans="8:8" x14ac:dyDescent="0.3">
+      <c r="H83">
+        <f>SUM(H58:H80)</f>
+        <v>2.9698000000000011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix DCDC track layout
</commit_message>
<xml_diff>
--- a/ESP32 Plotter Controller JLCPCB-LCSC BOM.xlsx
+++ b/ESP32 Plotter Controller JLCPCB-LCSC BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/635c63a8a9b49b7f/Code/ESP32_Plotter_Controller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="521" documentId="8_{D55F54B1-64B4-46E1-9F7C-A5FE78793489}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A5CE3CC6-27FB-43B9-AF21-B649572EF67A}"/>
+  <xr:revisionPtr revIDLastSave="547" documentId="8_{D55F54B1-64B4-46E1-9F7C-A5FE78793489}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F538A7CB-7DD5-4E87-A2F1-4D91FD7555E8}"/>
   <bookViews>
-    <workbookView xWindow="-37580" yWindow="-12810" windowWidth="37690" windowHeight="21820" xr2:uid="{9EA36A07-8613-46A5-ADBE-75DCC70AAE57}"/>
+    <workbookView xWindow="-34220" yWindow="-10060" windowWidth="15750" windowHeight="15950" xr2:uid="{9EA36A07-8613-46A5-ADBE-75DCC70AAE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="163">
   <si>
     <t>ESP32 Plotter Controller parts cross check</t>
   </si>
@@ -511,6 +511,18 @@
   </si>
   <si>
     <t>Component Order BOM (lcsc.com)</t>
+  </si>
+  <si>
+    <t>Ordered?</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Move capacitor nearer the dcdc chip, keep inductor feedback as short as possible, don't route under the inductor, connect en pin to via and leave floating</t>
   </si>
 </sst>
 </file>
@@ -869,10 +881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BC7673F-706C-49DA-BE28-CCAA818D7664}">
-  <dimension ref="B2:M83"/>
+  <dimension ref="A2:M84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C81" sqref="C81"/>
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2063,7 +2075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>122</v>
       </c>
@@ -2074,7 +2086,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>123</v>
       </c>
@@ -2085,18 +2097,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K52">
         <f>SUM(K5:K50)</f>
         <v>12.846600000000002</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>159</v>
+      </c>
       <c r="B57" t="s">
         <v>127</v>
       </c>
@@ -2119,7 +2134,10 @@
         <v>156</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>14</v>
+      </c>
       <c r="B58" t="s">
         <v>39</v>
       </c>
@@ -2140,7 +2158,10 @@
         <v>0.14879999999999999</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>160</v>
+      </c>
       <c r="B59" t="s">
         <v>120</v>
       </c>
@@ -2161,7 +2182,10 @@
         <v>0.1023</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>161</v>
+      </c>
       <c r="B60" t="s">
         <v>17</v>
       </c>
@@ -2182,7 +2206,10 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>160</v>
+      </c>
       <c r="B61" t="s">
         <v>31</v>
       </c>
@@ -2203,7 +2230,10 @@
         <v>3.4200000000000001E-2</v>
       </c>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>160</v>
+      </c>
       <c r="B62" t="s">
         <v>30</v>
       </c>
@@ -2224,7 +2254,10 @@
         <v>3.4200000000000001E-2</v>
       </c>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>160</v>
+      </c>
       <c r="B63" t="s">
         <v>36</v>
       </c>
@@ -2245,7 +2278,10 @@
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>160</v>
+      </c>
       <c r="B64" t="s">
         <v>42</v>
       </c>
@@ -2266,7 +2302,10 @@
         <v>3.9800000000000002E-2</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>160</v>
+      </c>
       <c r="B65" t="s">
         <v>44</v>
       </c>
@@ -2287,7 +2326,10 @@
         <v>0.34499999999999997</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>161</v>
+      </c>
       <c r="B66" t="s">
         <v>48</v>
       </c>
@@ -2308,7 +2350,10 @@
         <v>3.78E-2</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>160</v>
+      </c>
       <c r="B67" t="s">
         <v>26</v>
       </c>
@@ -2329,7 +2374,10 @@
         <v>0.17799999999999999</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>160</v>
+      </c>
       <c r="B68" t="s">
         <v>57</v>
       </c>
@@ -2350,7 +2398,10 @@
         <v>0.2238</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>160</v>
+      </c>
       <c r="B69" t="s">
         <v>60</v>
       </c>
@@ -2371,7 +2422,10 @@
         <v>0.4476</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>160</v>
+      </c>
       <c r="B70" t="s">
         <v>62</v>
       </c>
@@ -2392,7 +2446,10 @@
         <v>0.14460000000000001</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>161</v>
+      </c>
       <c r="B71" t="s">
         <v>119</v>
       </c>
@@ -2416,7 +2473,10 @@
         <v>0.2268</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>160</v>
+      </c>
       <c r="B72" t="s">
         <v>81</v>
       </c>
@@ -2440,7 +2500,10 @@
         <v>8.0799999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>160</v>
+      </c>
       <c r="B73" t="s">
         <v>126</v>
       </c>
@@ -2464,7 +2527,10 @@
         <v>0.1255</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>160</v>
+      </c>
       <c r="B74" t="s">
         <v>144</v>
       </c>
@@ -2488,7 +2554,10 @@
         <v>1.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>160</v>
+      </c>
       <c r="B75" t="s">
         <v>94</v>
       </c>
@@ -2512,7 +2581,10 @@
         <v>0.30330000000000001</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>160</v>
+      </c>
       <c r="B76" t="s">
         <v>98</v>
       </c>
@@ -2536,7 +2608,10 @@
         <v>6.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>161</v>
+      </c>
       <c r="B77" t="s">
         <v>150</v>
       </c>
@@ -2560,7 +2635,10 @@
         <v>0.20319999999999999</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>160</v>
+      </c>
       <c r="B78" t="s">
         <v>102</v>
       </c>
@@ -2584,7 +2662,10 @@
         <v>2.5999999999999999E-3</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>160</v>
+      </c>
       <c r="B79" t="s">
         <v>108</v>
       </c>
@@ -2608,7 +2689,10 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>160</v>
+      </c>
       <c r="B80" t="s">
         <v>115</v>
       </c>
@@ -2632,15 +2716,20 @@
         <v>0.23200000000000001</v>
       </c>
     </row>
-    <row r="82" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H82" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="83" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H83">
         <f>SUM(H58:H80)</f>
         <v>2.9698000000000011</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>